<commit_message>
may revision w/o new cbo
</commit_message>
<xml_diff>
--- a/data/cbo-projections.xlsx
+++ b/data/cbo-projections.xlsx
@@ -624,7 +624,7 @@
         <v>112.989</v>
       </c>
       <c r="H2">
-        <v>1.112827607409115</v>
+        <v>1.112827607409116</v>
       </c>
       <c r="I2">
         <v>1.158086067989782</v>
@@ -900,7 +900,7 @@
         <v>-0.007845261121856906</v>
       </c>
       <c r="AF4">
-        <v>2.438421052631579</v>
+        <v>2.43842105263158</v>
       </c>
       <c r="AG4">
         <v>-0.09956343886425356</v>
@@ -1275,7 +1275,7 @@
         <v>0.01477006910026257</v>
       </c>
       <c r="AC7">
-        <v>0.004638171381713851</v>
+        <v>0.004638171381713852</v>
       </c>
       <c r="AD7">
         <v>0.008700317431931115</v>
@@ -1553,7 +1553,7 @@
         <v>0.02091044906382988</v>
       </c>
       <c r="AB9">
-        <v>0.01086876123098079</v>
+        <v>0.0108687612309808</v>
       </c>
       <c r="AC9">
         <v>0.004995583173413642</v>
@@ -1592,7 +1592,7 @@
         <v>0.01341818361205682</v>
       </c>
       <c r="AO9">
-        <v>-0.602424064437252</v>
+        <v>-0.6024240644372521</v>
       </c>
       <c r="AP9">
         <v>0</v>
@@ -1668,7 +1668,7 @@
         <v>13968.1</v>
       </c>
       <c r="R10">
-        <v>0.01265029143343654</v>
+        <v>0.01265029143343655</v>
       </c>
       <c r="S10">
         <v>0.009392532637389817</v>
@@ -1780,31 +1780,31 @@
         <v>118.436</v>
       </c>
       <c r="H11">
-        <v>1.172344903764031</v>
+        <v>1.158264947245018</v>
       </c>
       <c r="I11">
-        <v>1.273432609555655</v>
+        <v>1.253622839535892</v>
       </c>
       <c r="J11">
-        <v>1.169084677044773</v>
+        <v>1.154769676155877</v>
       </c>
       <c r="K11">
         <v>0.00472518429915425</v>
       </c>
       <c r="L11">
-        <v>0.01705852500181471</v>
+        <v>0.004843570372557782</v>
       </c>
       <c r="M11">
-        <v>0.02388085658353312</v>
+        <v>0.00795316308459304</v>
       </c>
       <c r="N11">
-        <v>0.01705852500181249</v>
+        <v>0.004605027000056161</v>
       </c>
       <c r="O11">
         <v>115.476</v>
       </c>
       <c r="P11">
-        <v>16476.1441705274</v>
+        <v>16274.4</v>
       </c>
       <c r="Q11">
         <v>14093.2</v>
@@ -1840,31 +1840,31 @@
         <v>0.01210694551131142</v>
       </c>
       <c r="AB11">
-        <v>0.0100889550024934</v>
+        <v>0.01008895500249341</v>
       </c>
       <c r="AC11">
         <v>0.005296934914037932</v>
       </c>
       <c r="AD11">
-        <v>0.004602120977494017</v>
+        <v>0.004602120977494018</v>
       </c>
       <c r="AE11">
-        <v>0.00539661609576858</v>
+        <v>0.005396616095768581</v>
       </c>
       <c r="AF11">
         <v>-0.1095682360598829</v>
       </c>
       <c r="AG11">
-        <v>0.02616742467161193</v>
+        <v>0.01360239162929733</v>
       </c>
       <c r="AH11">
         <v>0.01126120683405407</v>
       </c>
       <c r="AI11">
-        <v>0.01989821816493498</v>
+        <v>0.007649158592554883</v>
       </c>
       <c r="AJ11">
-        <v>0.02948152154596584</v>
+        <v>0.0134667029930331</v>
       </c>
       <c r="AK11">
         <v>0.008956121448156829</v>
@@ -1891,7 +1891,7 @@
         <v>-0.04186576482736426</v>
       </c>
       <c r="AS11">
-        <v>-0.09338911510963221</v>
+        <v>-0.09338911510963222</v>
       </c>
       <c r="AT11">
         <v>0.04595568398863437</v>
@@ -1928,31 +1928,31 @@
         <v>119.039</v>
       </c>
       <c r="H12">
-        <v>1.189547712538471</v>
+        <v>1.163395810363837</v>
       </c>
       <c r="I12">
-        <v>1.298171007879712</v>
+        <v>1.264110297285653</v>
       </c>
       <c r="J12">
-        <v>1.186239645753866</v>
+        <v>1.160652920962199</v>
       </c>
       <c r="K12">
         <v>0.005091357357560167</v>
       </c>
       <c r="L12">
-        <v>0.01467384616865486</v>
+        <v>0.004429783644081864</v>
       </c>
       <c r="M12">
-        <v>0.01942654690827261</v>
+        <v>0.008365720070674376</v>
       </c>
       <c r="N12">
-        <v>0.01467384616866019</v>
+        <v>0.005094734411374313</v>
       </c>
       <c r="O12">
         <v>116.065</v>
       </c>
       <c r="P12">
-        <v>16845.5519614215</v>
+        <v>16482.2</v>
       </c>
       <c r="Q12">
         <v>14200.8</v>
@@ -1976,7 +1976,7 @@
         <v>0.008349389265587703</v>
       </c>
       <c r="X12">
-        <v>0.07053784555518527</v>
+        <v>0.07053784555518528</v>
       </c>
       <c r="Y12">
         <v>0.03674283345286411</v>
@@ -2003,16 +2003,16 @@
         <v>-0.06944444444444453</v>
       </c>
       <c r="AG12">
-        <v>0.02242076708426111</v>
+        <v>0.01276851988398975</v>
       </c>
       <c r="AH12">
         <v>0.009224078189595586</v>
       </c>
       <c r="AI12">
-        <v>0.01147696930865671</v>
+        <v>0.001265182186234837</v>
       </c>
       <c r="AJ12">
-        <v>0.02521790661821344</v>
+        <v>0.01409424325050868</v>
       </c>
       <c r="AK12">
         <v>0.007634887747282271</v>
@@ -2024,7 +2024,7 @@
         <v>-0.003150644783118328</v>
       </c>
       <c r="AN12">
-        <v>0.005680997544653676</v>
+        <v>0.005680997544653677</v>
       </c>
       <c r="AO12">
         <v>0.2027464249937341</v>
@@ -2076,31 +2076,31 @@
         <v>119.672</v>
       </c>
       <c r="H13">
-        <v>1.204146120931274</v>
+        <v>1.169154596511972</v>
       </c>
       <c r="I13">
-        <v>1.320315890474254</v>
+        <v>1.274804052762378</v>
       </c>
       <c r="J13">
-        <v>1.200797456775579</v>
+        <v>1.166586379027472</v>
       </c>
       <c r="K13">
         <v>0.00531758499315349</v>
       </c>
       <c r="L13">
-        <v>0.01227223442904202</v>
+        <v>0.00494998013301573</v>
       </c>
       <c r="M13">
-        <v>0.01705852500181115</v>
+        <v>0.00845951140473078</v>
       </c>
       <c r="N13">
-        <v>0.01227223442903957</v>
+        <v>0.005112172603980447</v>
       </c>
       <c r="O13">
         <v>116.658</v>
       </c>
       <c r="P13">
-        <v>17199.622372125</v>
+        <v>16709.6</v>
       </c>
       <c r="Q13">
         <v>14323.5</v>
@@ -2115,7 +2115,7 @@
         <v>-0.6533418960601727</v>
       </c>
       <c r="U13">
-        <v>-0.06754446627567789</v>
+        <v>-0.0675444662756779</v>
       </c>
       <c r="V13">
         <v>0.04208737571233967</v>
@@ -2151,16 +2151,16 @@
         <v>-0.03587326525268397</v>
       </c>
       <c r="AG13">
-        <v>0.02101862922119535</v>
+        <v>0.01379670189659144</v>
       </c>
       <c r="AH13">
         <v>0.006227357753415541</v>
       </c>
       <c r="AI13">
-        <v>0.006840711230709173</v>
+        <v>-0.0004422542330048129</v>
       </c>
       <c r="AJ13">
-        <v>0.01876262995537825</v>
+        <v>0.01014920851321666</v>
       </c>
       <c r="AK13">
         <v>0.008640358289673911</v>
@@ -2224,31 +2224,31 @@
         <v>120.331</v>
       </c>
       <c r="H14">
-        <v>1.216011062205169</v>
+        <v>1.175033417495916</v>
       </c>
       <c r="I14">
-        <v>1.341267039027538</v>
+        <v>1.285461755291195</v>
       </c>
       <c r="J14">
-        <v>1.212629402300156</v>
+        <v>1.172554319575839</v>
       </c>
       <c r="K14">
         <v>0.005506718363527119</v>
       </c>
       <c r="L14">
-        <v>0.009853406548964605</v>
+        <v>0.00502826657952915</v>
       </c>
       <c r="M14">
-        <v>0.01586828478278668</v>
+        <v>0.008360267215751893</v>
       </c>
       <c r="N14">
-        <v>0.009853406548968602</v>
+        <v>0.005115729667049873</v>
       </c>
       <c r="O14">
         <v>117.255</v>
       </c>
       <c r="P14">
-        <v>17496.4233310878</v>
+        <v>16918.2</v>
       </c>
       <c r="Q14">
         <v>14428.5</v>
@@ -2299,16 +2299,16 @@
         <v>-0.01222161868549698</v>
       </c>
       <c r="AG14">
-        <v>0.01725624856995811</v>
+        <v>0.01248384162397676</v>
       </c>
       <c r="AH14">
         <v>0.005482868975903443</v>
       </c>
       <c r="AI14">
-        <v>0.004928020439576963</v>
+        <v>0.0001264142595285289</v>
       </c>
       <c r="AJ14">
-        <v>0.01620813748750249</v>
+        <v>0.008697608157756553</v>
       </c>
       <c r="AK14">
         <v>0.007330610535134507</v>
@@ -2317,7 +2317,7 @@
         <v>-0.001624648234645587</v>
       </c>
       <c r="AM14">
-        <v>-0.004877327815548393</v>
+        <v>-0.004877327815548394</v>
       </c>
       <c r="AN14">
         <v>0.0003345440642323894</v>
@@ -2372,31 +2372,31 @@
         <v>120.992</v>
       </c>
       <c r="H15">
-        <v>1.227992913569121</v>
+        <v>1.181046676096181</v>
       </c>
       <c r="I15">
-        <v>1.360948585229321</v>
+        <v>1.296174236996705</v>
       </c>
       <c r="J15">
-        <v>1.224577932794252</v>
+        <v>1.178627795582205</v>
       </c>
       <c r="K15">
         <v>0.005493181308224848</v>
       </c>
       <c r="L15">
-        <v>0.009853406548970156</v>
+        <v>0.005117521349375931</v>
       </c>
       <c r="M15">
-        <v>0.01467384616865908</v>
+        <v>0.008333567032558609</v>
       </c>
       <c r="N15">
-        <v>0.00985340654896838</v>
+        <v>0.005179696927441579</v>
       </c>
       <c r="O15">
         <v>117.862</v>
       </c>
       <c r="P15">
-        <v>17768.0135158782</v>
+        <v>17101.3</v>
       </c>
       <c r="Q15">
         <v>14509.5</v>
@@ -2447,16 +2447,16 @@
         <v>0.006873797085509947</v>
       </c>
       <c r="AG15">
-        <v>0.01552261165902613</v>
+        <v>0.01082266434963519</v>
       </c>
       <c r="AH15">
         <v>0.006412506728451506</v>
       </c>
       <c r="AI15">
-        <v>0.00737864326246207</v>
+        <v>0.00265436390065088</v>
       </c>
       <c r="AJ15">
-        <v>0.01496470867293564</v>
+        <v>0.008622612056790491</v>
       </c>
       <c r="AK15">
         <v>0.00561388917766914</v>
@@ -2520,31 +2520,31 @@
         <v>121.658</v>
       </c>
       <c r="H16">
-        <v>1.238599636045654</v>
+        <v>1.18711793648427</v>
       </c>
       <c r="I16">
-        <v>1.379287604820847</v>
+        <v>1.306936361034253</v>
       </c>
       <c r="J16">
-        <v>1.235155158558754</v>
+        <v>1.184778955310903</v>
       </c>
       <c r="K16">
         <v>0.005504496165035677</v>
       </c>
       <c r="L16">
-        <v>0.008637445997717208</v>
+        <v>0.005140576160932886</v>
       </c>
       <c r="M16">
-        <v>0.01347517444124158</v>
+        <v>0.008302991781787172</v>
       </c>
       <c r="N16">
-        <v>0.008637445997713655</v>
+        <v>0.005218916227628823</v>
       </c>
       <c r="O16">
         <v>118.477</v>
       </c>
       <c r="P16">
-        <v>18006.7094790488</v>
+        <v>17272.3</v>
       </c>
       <c r="Q16">
         <v>14578.5</v>
@@ -2595,22 +2595,22 @@
         <v>0.01529219006007643</v>
       </c>
       <c r="AG16">
-        <v>0.01343402642942015</v>
+        <v>0.009999239823873074</v>
       </c>
       <c r="AH16">
         <v>0.00739483291863352</v>
       </c>
       <c r="AI16">
-        <v>0.007210801802529643</v>
+        <v>0.00371887803340698</v>
       </c>
       <c r="AJ16">
-        <v>0.01468532295158353</v>
+        <v>0.009506964404156326</v>
       </c>
       <c r="AK16">
         <v>0.004755505013956274</v>
       </c>
       <c r="AL16">
-        <v>0.0002035593811793301</v>
+        <v>0.0002035593811793302</v>
       </c>
       <c r="AM16">
         <v>-0.001414427157001352</v>
@@ -2619,7 +2619,7 @@
         <v>0.001194058365572959</v>
       </c>
       <c r="AO16">
-        <v>0.0104497170039286</v>
+        <v>0.01044971700392861</v>
       </c>
       <c r="AP16">
         <v>0</v>
@@ -2668,31 +2668,31 @@
         <v>122.323</v>
       </c>
       <c r="H17">
-        <v>1.247786418450075</v>
+        <v>1.193495449798598</v>
       </c>
       <c r="I17">
-        <v>1.396214545652274</v>
+        <v>1.317869743491942</v>
       </c>
       <c r="J17">
-        <v>1.244316393026423</v>
+        <v>1.190987607960946</v>
       </c>
       <c r="K17">
         <v>0.005466142793733253</v>
       </c>
       <c r="L17">
-        <v>0.007417071777729989</v>
+        <v>0.005372265988343949</v>
       </c>
       <c r="M17">
-        <v>0.01227223442903735</v>
+        <v>0.008365657872612564</v>
       </c>
       <c r="N17">
-        <v>0.007417071777733764</v>
+        <v>0.005240346836186127</v>
       </c>
       <c r="O17">
         <v>119.098</v>
       </c>
       <c r="P17">
-        <v>18224.8800504615</v>
+        <v>17443.8</v>
       </c>
       <c r="Q17">
         <v>14646.5</v>
@@ -2701,7 +2701,7 @@
         <v>-0.01574918805999381</v>
       </c>
       <c r="S17">
-        <v>0.03720972619024931</v>
+        <v>0.03720972619024932</v>
       </c>
       <c r="T17">
         <v>-0.1097645610238424</v>
@@ -2743,16 +2743,16 @@
         <v>0.0153308230231306</v>
       </c>
       <c r="AG17">
-        <v>0.01211607104932444</v>
+        <v>0.009929192985300261</v>
       </c>
       <c r="AH17">
         <v>0.007386717758131267</v>
       </c>
       <c r="AI17">
-        <v>0.006816256467291337</v>
+        <v>0.004772670183371019</v>
       </c>
       <c r="AJ17">
-        <v>0.01285172430658488</v>
+        <v>0.008942911373923224</v>
       </c>
       <c r="AK17">
         <v>0.004664403059299715</v>
@@ -2816,31 +2816,31 @@
         <v>122.988</v>
       </c>
       <c r="H18">
-        <v>1.257041339878998</v>
+        <v>1.199955250596659</v>
       </c>
       <c r="I18">
-        <v>1.413349217869756</v>
+        <v>1.32864833960646</v>
       </c>
       <c r="J18">
-        <v>1.253545577027709</v>
+        <v>1.19723931594873</v>
       </c>
       <c r="K18">
         <v>0.005436426510141201</v>
       </c>
       <c r="L18">
-        <v>0.007417071777731765</v>
+        <v>0.005412505593675565</v>
       </c>
       <c r="M18">
-        <v>0.01227223442904091</v>
+        <v>0.008178802319232181</v>
       </c>
       <c r="N18">
-        <v>0.007417071777732431</v>
+        <v>0.005249179711019236</v>
       </c>
       <c r="O18">
         <v>119.724</v>
       </c>
       <c r="P18">
-        <v>18435.268028558</v>
+        <v>17607.2</v>
       </c>
       <c r="Q18">
         <v>14706.5</v>
@@ -2849,7 +2849,7 @@
         <v>0.003535771276076849</v>
       </c>
       <c r="S18">
-        <v>0.02020444450621794</v>
+        <v>0.02020444450621795</v>
       </c>
       <c r="T18">
         <v>0.01727635461373378</v>
@@ -2891,16 +2891,16 @@
         <v>0.01589403973509929</v>
       </c>
       <c r="AG18">
-        <v>0.01154399795850347</v>
+        <v>0.00936722503124332</v>
       </c>
       <c r="AH18">
         <v>0.007676267729886943</v>
       </c>
       <c r="AI18">
-        <v>0.007567365239133705</v>
+        <v>0.005562500000000137</v>
       </c>
       <c r="AJ18">
-        <v>0.01299618234152455</v>
+        <v>0.008899822727108209</v>
       </c>
       <c r="AK18">
         <v>0.004096541835933554</v>
@@ -2964,31 +2964,31 @@
         <v>123.65</v>
       </c>
       <c r="H19">
-        <v>1.266364905724463</v>
+        <v>1.20659307875895</v>
       </c>
       <c r="I19">
-        <v>1.428987913537465</v>
+        <v>1.339472682276794</v>
       </c>
       <c r="J19">
-        <v>1.262843214549183</v>
+        <v>1.20348986921461</v>
       </c>
       <c r="K19">
         <v>0.005382638956646257</v>
       </c>
       <c r="L19">
-        <v>0.007417071777737094</v>
+        <v>0.005531729753247339</v>
       </c>
       <c r="M19">
-        <v>0.01106499049914933</v>
+        <v>0.008146883074824807</v>
       </c>
       <c r="N19">
-        <v>0.007417071777733319</v>
+        <v>0.005220805216312741</v>
       </c>
       <c r="O19">
         <v>120.348</v>
       </c>
       <c r="P19">
-        <v>18635.7773171023</v>
+        <v>17759.9</v>
       </c>
       <c r="Q19">
         <v>14757</v>
@@ -3039,16 +3039,16 @@
         <v>0.01955671447196883</v>
       </c>
       <c r="AG19">
-        <v>0.01087639671057095</v>
+        <v>0.008672588486528188</v>
       </c>
       <c r="AH19">
         <v>0.007890667636892834</v>
       </c>
       <c r="AI19">
-        <v>0.007417071777737094</v>
+        <v>0.005531729753247561</v>
       </c>
       <c r="AJ19">
-        <v>0.01217292774158474</v>
+        <v>0.009251622619858679</v>
       </c>
       <c r="AK19">
         <v>0.003433855778057326</v>
@@ -3112,31 +3112,31 @@
         <v>124.311</v>
       </c>
       <c r="H20">
-        <v>1.274206549158844</v>
+        <v>1.213124533929903</v>
       </c>
       <c r="I20">
-        <v>1.443068312403112</v>
+        <v>1.350308788598575</v>
       </c>
       <c r="J20">
-        <v>1.270663050804327</v>
+        <v>1.209772171728767</v>
       </c>
       <c r="K20">
         <v>0.005345733926405138</v>
       </c>
       <c r="L20">
-        <v>0.006192246325631645</v>
+        <v>0.005413138270004891</v>
       </c>
       <c r="M20">
-        <v>0.009853406548968602</v>
+        <v>0.008089830024276212</v>
       </c>
       <c r="N20">
-        <v>0.006192246325633644</v>
+        <v>0.005220070957686174</v>
       </c>
       <c r="O20">
         <v>120.977</v>
       </c>
       <c r="P20">
-        <v>18817.7573845816</v>
+        <v>17916</v>
       </c>
       <c r="Q20">
         <v>14809.4</v>
@@ -3187,16 +3187,16 @@
         <v>0.01585677749360603</v>
       </c>
       <c r="AG20">
-        <v>0.009765091328511222</v>
+        <v>0.008789463904639083</v>
       </c>
       <c r="AH20">
         <v>0.008325248742187874</v>
       </c>
       <c r="AI20">
-        <v>0.006342334667863936</v>
+        <v>0.005563110396835214</v>
       </c>
       <c r="AJ20">
-        <v>0.01167971672643198</v>
+        <v>0.00991295079054888</v>
       </c>
       <c r="AK20">
         <v>0.003550857220302239</v>
@@ -3260,31 +3260,31 @@
         <v>124.973</v>
       </c>
       <c r="H21">
-        <v>1.274206549158847</v>
+        <v>1.219819551114757</v>
       </c>
       <c r="I21">
-        <v>1.44306831240311</v>
+        <v>1.361115061868866</v>
       </c>
       <c r="J21">
-        <v>1.270663050804327</v>
+        <v>1.21607604133032</v>
       </c>
       <c r="K21">
         <v>0.005325353347652273</v>
       </c>
       <c r="L21">
-        <v>2.442490654175344e-15</v>
+        <v>0.005518821025872089</v>
       </c>
       <c r="M21">
-        <v>-1.221245327087672e-15</v>
+        <v>0.008002816364327092</v>
       </c>
       <c r="N21">
-        <v>-2.220446049250313e-16</v>
+        <v>0.00521079071652375</v>
       </c>
       <c r="O21">
         <v>121.608</v>
       </c>
       <c r="P21">
-        <v>18889.1686480368</v>
+        <v>18077.7</v>
       </c>
       <c r="Q21">
         <v>14865.6</v>
@@ -3335,16 +3335,16 @@
         <v>0.01233635448136949</v>
       </c>
       <c r="AG21">
-        <v>0.003794887031209671</v>
+        <v>0.009025452109846066</v>
       </c>
       <c r="AH21">
         <v>0.008435514185983983</v>
       </c>
       <c r="AI21">
-        <v>7.457121551324164e-05</v>
+        <v>0.005593803786575036</v>
       </c>
       <c r="AJ21">
-        <v>0.002042755344417113</v>
+        <v>0.01006191950464386</v>
       </c>
       <c r="AK21">
         <v>0.003794887031209893</v>
@@ -3353,7 +3353,7 @@
         <v>0.001304953021691313</v>
       </c>
       <c r="AM21">
-        <v>7.457121551079915e-05</v>
+        <v>7.457121551079915e-005</v>
       </c>
       <c r="AN21">
         <v>0.002042755344418223</v>
@@ -3408,31 +3408,31 @@
         <v>125.64</v>
       </c>
       <c r="H22">
-        <v>1.274206549158844</v>
+        <v>1.22662192393736</v>
       </c>
       <c r="I22">
-        <v>1.443068312403109</v>
+        <v>1.372007192202139</v>
       </c>
       <c r="J22">
-        <v>1.270663050804324</v>
+        <v>1.222406266136441</v>
       </c>
       <c r="K22">
         <v>0.005337152825010127</v>
       </c>
       <c r="L22">
-        <v>-2.442490654175344e-15</v>
+        <v>0.005576540248422024</v>
       </c>
       <c r="M22">
-        <v>-7.771561172376096e-16</v>
+        <v>0.008002358241717689</v>
       </c>
       <c r="N22">
-        <v>-2.220446049250313e-15</v>
+        <v>0.005205451461075317</v>
       </c>
       <c r="O22">
         <v>122.24</v>
       </c>
       <c r="P22">
-        <v>18948.000347289</v>
+        <v>18228.4</v>
       </c>
       <c r="Q22">
         <v>14911.9</v>
@@ -3465,13 +3465,13 @@
         <v>0.008104571219532453</v>
       </c>
       <c r="AA22">
-        <v>0.002752470861042688</v>
+        <v>0.002752470861042689</v>
       </c>
       <c r="AB22">
         <v>0.01003821365425206</v>
       </c>
       <c r="AC22">
-        <v>0.004682159782861905</v>
+        <v>0.004682159782861906</v>
       </c>
       <c r="AD22">
         <v>0.005197026511413627</v>
@@ -3483,16 +3483,16 @@
         <v>0.01517035563292701</v>
       </c>
       <c r="AG22">
-        <v>0.00311457324292097</v>
+        <v>0.008336237463836715</v>
       </c>
       <c r="AH22">
         <v>0.008342763318467394</v>
       </c>
       <c r="AI22">
-        <v>-7.456565506180901e-05</v>
+        <v>0.005501558774986259</v>
       </c>
       <c r="AJ22">
-        <v>0.001943772815625078</v>
+        <v>0.009961685823754785</v>
       </c>
       <c r="AK22">
         <v>0.003114573242923191</v>
@@ -3501,7 +3501,7 @@
         <v>0.001216368849372929</v>
       </c>
       <c r="AM22">
-        <v>-7.45656550592555e-05</v>
+        <v>-7.45656550592555e-005</v>
       </c>
       <c r="AN22">
         <v>0.001943772815625966</v>
@@ -3513,7 +3513,7 @@
         <v>0</v>
       </c>
       <c r="AQ22">
-        <v>0.06095262562726766</v>
+        <v>0.06095262562726767</v>
       </c>
       <c r="AR22">
         <v>0.01634348802504726</v>
@@ -3556,31 +3556,31 @@
         <v>126.304</v>
       </c>
       <c r="H23">
-        <v>1.274206549158846</v>
+        <v>1.233492323744224</v>
       </c>
       <c r="I23">
-        <v>1.443068312403112</v>
+        <v>1.382998819362456</v>
       </c>
       <c r="J23">
-        <v>1.270663050804324</v>
+        <v>1.228728344168209</v>
       </c>
       <c r="K23">
         <v>0.005284941101560081</v>
       </c>
       <c r="L23">
-        <v>1.77635683940025e-15</v>
+        <v>0.005601073707218962</v>
       </c>
       <c r="M23">
-        <v>2.442490654175344e-15</v>
+        <v>0.008011348062013424</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>0.005171830517319842</v>
       </c>
       <c r="O23">
         <v>122.872</v>
       </c>
       <c r="P23">
-        <v>19018.1409476934</v>
+        <v>18390.5</v>
       </c>
       <c r="Q23">
         <v>14967.1</v>
@@ -3631,16 +3631,16 @@
         <v>0.01445369916707495</v>
       </c>
       <c r="AG23">
-        <v>0.003701741562108118</v>
+        <v>0.00889271685940618</v>
       </c>
       <c r="AH23">
         <v>0.008581802178457387</v>
       </c>
       <c r="AI23">
-        <v>0.0005965697240881696</v>
+        <v>0.006200984862301473</v>
       </c>
       <c r="AJ23">
-        <v>0.001940001892687171</v>
+        <v>0.009966891985101478</v>
       </c>
       <c r="AK23">
         <v>0.003701741562108118</v>
@@ -3704,31 +3704,31 @@
         <v>126.974</v>
       </c>
       <c r="H24">
-        <v>1.274206549158844</v>
+        <v>1.240262158337678</v>
       </c>
       <c r="I24">
-        <v>1.443068312403111</v>
+        <v>1.393976528255644</v>
       </c>
       <c r="J24">
-        <v>1.270663050804324</v>
+        <v>1.235117185940349</v>
       </c>
       <c r="K24">
-        <v>0.005304661768431806</v>
+        <v>0.005304661768431807</v>
       </c>
       <c r="L24">
-        <v>-1.77635683940025e-15</v>
+        <v>0.005488347566609875</v>
       </c>
       <c r="M24">
-        <v>-1.110223024625157e-15</v>
+        <v>0.007937612628077906</v>
       </c>
       <c r="N24">
-        <v>2.220446049250313e-16</v>
+        <v>0.005199555949419343</v>
       </c>
       <c r="O24">
         <v>123.511</v>
       </c>
       <c r="P24">
-        <v>19094.7619296569</v>
+        <v>18560.6</v>
       </c>
       <c r="Q24">
         <v>15027.4</v>
@@ -3779,16 +3779,16 @@
         <v>0.008935039845447967</v>
       </c>
       <c r="AG24">
-        <v>0.004028836581568829</v>
+        <v>0.009249340692205177</v>
       </c>
       <c r="AH24">
         <v>0.008596051052689013</v>
       </c>
       <c r="AI24">
-        <v>0.0006707407959440914</v>
+        <v>0.006162769621171016</v>
       </c>
       <c r="AJ24">
-        <v>0.001983471074379128</v>
+        <v>0.009936827727505593</v>
       </c>
       <c r="AK24">
         <v>0.004028836581568829</v>
@@ -3852,31 +3852,31 @@
         <v>127.646</v>
       </c>
       <c r="H25">
-        <v>1.274206549158846</v>
+        <v>1.247264607368813</v>
       </c>
       <c r="I25">
-        <v>1.443068312403109</v>
+        <v>1.405004939084623</v>
       </c>
       <c r="J25">
-        <v>1.270663050804325</v>
+        <v>1.241533372664179</v>
       </c>
       <c r="K25">
         <v>0.005292422070660052</v>
       </c>
       <c r="L25">
-        <v>1.77635683940025e-15</v>
+        <v>0.005645942661445247</v>
       </c>
       <c r="M25">
-        <v>-1.110223024625157e-15</v>
+        <v>0.007911475269084312</v>
       </c>
       <c r="N25">
-        <v>4.440892098500626e-16</v>
+        <v>0.005194799972720654</v>
       </c>
       <c r="O25">
         <v>124.153</v>
       </c>
       <c r="P25">
-        <v>19168.8415855188</v>
+        <v>18729.4</v>
       </c>
       <c r="Q25">
         <v>15085.7</v>
@@ -3924,19 +3924,19 @@
         <v>0.006020537443098606</v>
       </c>
       <c r="AF25">
-        <v>0.007659167065581673</v>
+        <v>0.007659167065581674</v>
       </c>
       <c r="AG25">
-        <v>0.003879579967260183</v>
+        <v>0.009094533581888609</v>
       </c>
       <c r="AH25">
         <v>0.008587683056090478</v>
       </c>
       <c r="AI25">
-        <v>0.0005958144038149538</v>
+        <v>0.006245120999219367</v>
       </c>
       <c r="AJ25">
-        <v>0.001979544704717062</v>
+        <v>0.009906681092777925</v>
       </c>
       <c r="AK25">
         <v>0.003879579967259961</v>
@@ -3951,7 +3951,7 @@
         <v>0.00197954470471795</v>
       </c>
       <c r="AO25">
-        <v>0.0002603289741658354</v>
+        <v>0.0002603289741658355</v>
       </c>
       <c r="AP25">
         <v>0</v>
@@ -4000,31 +4000,31 @@
         <v>128.32</v>
       </c>
       <c r="H26">
-        <v>1.274206549158849</v>
+        <v>1.254333110168861</v>
       </c>
       <c r="I26">
-        <v>1.443068312403113</v>
+        <v>1.416083751936529</v>
       </c>
       <c r="J26">
-        <v>1.270663050804323</v>
+        <v>1.247989488557582</v>
       </c>
       <c r="K26">
         <v>0.005280228130924547</v>
       </c>
       <c r="L26">
-        <v>1.77635683940025e-15</v>
+        <v>0.00566720386218611</v>
       </c>
       <c r="M26">
-        <v>2.442490654175344e-15</v>
+        <v>0.00788524833167048</v>
       </c>
       <c r="N26">
-        <v>-9.992007221626409e-16</v>
+        <v>0.005200114661073618</v>
       </c>
       <c r="O26">
         <v>124.799</v>
       </c>
       <c r="P26">
-        <v>19244.7001696518</v>
+        <v>18901.3</v>
       </c>
       <c r="Q26">
         <v>15145.4</v>
@@ -4075,22 +4075,22 @@
         <v>0.009263657957244487</v>
       </c>
       <c r="AG26">
-        <v>0.003957390111163805</v>
+        <v>0.009178083654574953</v>
       </c>
       <c r="AH26">
         <v>0.008557457212713837</v>
       </c>
       <c r="AI26">
-        <v>0.0005954596203963103</v>
+        <v>0.00626603807364079</v>
       </c>
       <c r="AJ26">
-        <v>0.001975633849195635</v>
+        <v>0.009876460544377075</v>
       </c>
       <c r="AK26">
         <v>0.003957390111164916</v>
       </c>
       <c r="AL26">
-        <v>0.001468682505399554</v>
+        <v>0.001468682505399555</v>
       </c>
       <c r="AM26">
         <v>0.0005954596203945339</v>
@@ -4148,31 +4148,31 @@
         <v>129.002</v>
       </c>
       <c r="H27">
-        <v>1.274206549158844</v>
+        <v>1.26143207673433</v>
       </c>
       <c r="I27">
-        <v>1.443068312403111</v>
+        <v>1.427279542685784</v>
       </c>
       <c r="J27">
-        <v>1.270663050804325</v>
+        <v>1.254541864139021</v>
       </c>
       <c r="K27">
         <v>0.005314837905237013</v>
       </c>
       <c r="L27">
-        <v>-3.33066907387547e-15</v>
+        <v>0.005659554473940842</v>
       </c>
       <c r="M27">
-        <v>-8.881784197001252e-16</v>
+        <v>0.007906164260372828</v>
       </c>
       <c r="N27">
-        <v>1.110223024625157e-15</v>
+        <v>0.005250345168381188</v>
       </c>
       <c r="O27">
         <v>125.454</v>
       </c>
       <c r="P27">
-        <v>19303.9130678193</v>
+        <v>19059</v>
       </c>
       <c r="Q27">
         <v>15192</v>
@@ -4214,7 +4214,7 @@
         <v>0.00430355391758197</v>
       </c>
       <c r="AD27">
-        <v>0.005248439490700862</v>
+        <v>0.005248439490700863</v>
       </c>
       <c r="AE27">
         <v>0.006056618416169002</v>
@@ -4223,19 +4223,19 @@
         <v>0.01317957166392092</v>
       </c>
       <c r="AG27">
-        <v>0.003076841813356879</v>
+        <v>0.008343341463285636</v>
       </c>
       <c r="AH27">
         <v>0.008527379053694828</v>
       </c>
       <c r="AI27">
-        <v>0.0004463289444289753</v>
+        <v>0.006108409441347273</v>
       </c>
       <c r="AJ27">
-        <v>0.001924792263273245</v>
+        <v>0.009846174247447159</v>
       </c>
       <c r="AK27">
-        <v>0.00307684181335599</v>
+        <v>0.003076841813355991</v>
       </c>
       <c r="AL27">
         <v>0.001409017713365657</v>
@@ -4296,31 +4296,31 @@
         <v>129.682</v>
       </c>
       <c r="H28">
-        <v>1.274206549158848</v>
+        <v>1.268599033816425</v>
       </c>
       <c r="I28">
-        <v>1.44306831240311</v>
+        <v>1.438525931814993</v>
       </c>
       <c r="J28">
-        <v>1.270663050804328</v>
+        <v>1.261049624198104</v>
       </c>
       <c r="K28">
         <v>0.00527123610486635</v>
       </c>
       <c r="L28">
-        <v>2.886579864025407e-15</v>
+        <v>0.005681603642623267</v>
       </c>
       <c r="M28">
-        <v>-1.110223024625157e-15</v>
+        <v>0.007879598069517657</v>
       </c>
       <c r="N28">
-        <v>2.220446049250313e-15</v>
+        <v>0.005187359820430837</v>
       </c>
       <c r="O28">
         <v>126.105</v>
       </c>
       <c r="P28">
-        <v>19391.2076194096</v>
+        <v>19244.5</v>
       </c>
       <c r="Q28">
         <v>15260.7</v>
@@ -4353,7 +4353,7 @@
         <v>0.009343381830958508</v>
       </c>
       <c r="AA28">
-        <v>0.004051653962850787</v>
+        <v>0.004051653962850788</v>
       </c>
       <c r="AB28">
         <v>0.009525039089957055</v>
@@ -4371,16 +4371,16 @@
         <v>0.006271777003484358</v>
       </c>
       <c r="AG28">
-        <v>0.004522116903635798</v>
+        <v>0.009732934571593521</v>
       </c>
       <c r="AH28">
         <v>0.008497448656854756</v>
       </c>
       <c r="AI28">
-        <v>0.0004461298237814493</v>
+        <v>0.006130268199233679</v>
       </c>
       <c r="AJ28">
-        <v>0.001921094555335845</v>
+        <v>0.009815830077804399</v>
       </c>
       <c r="AK28">
         <v>0.004522116903633577</v>
@@ -4395,7 +4395,7 @@
         <v>0.001921094555336955</v>
       </c>
       <c r="AO28">
-        <v>0.002306876975147309</v>
+        <v>0.00230687697514731</v>
       </c>
       <c r="AP28">
         <v>0</v>
@@ -4404,7 +4404,7 @@
         <v>0</v>
       </c>
       <c r="AR28">
-        <v>0.01628478684219536</v>
+        <v>0.01628478684219537</v>
       </c>
       <c r="AS28">
         <v>0.01193121498860017</v>
@@ -4444,31 +4444,31 @@
         <v>130.368</v>
       </c>
       <c r="H29">
-        <v>1.274206549158847</v>
+        <v>1.275813400683405</v>
       </c>
       <c r="I29">
-        <v>1.443068312403109</v>
+        <v>1.449890304812584</v>
       </c>
       <c r="J29">
-        <v>1.270663050804328</v>
+        <v>1.26759415071942</v>
       </c>
       <c r="K29">
-        <v>0.005289862895390351</v>
+        <v>0.005289862895390352</v>
       </c>
       <c r="L29">
-        <v>-8.881784197001252e-16</v>
+        <v>0.005686877157139669</v>
       </c>
       <c r="M29">
-        <v>-7.771561172376096e-16</v>
+        <v>0.00790001260752593</v>
       </c>
       <c r="N29">
-        <v>6.661338147750939e-16</v>
+        <v>0.005189745427724768</v>
       </c>
       <c r="O29">
         <v>126.759</v>
       </c>
       <c r="P29">
-        <v>19481.5517623218</v>
+        <v>19434.5</v>
       </c>
       <c r="Q29">
         <v>15331.8</v>
@@ -4489,7 +4489,7 @@
         <v>0.02037414911907698</v>
       </c>
       <c r="W29">
-        <v>0.008448152274435738</v>
+        <v>0.008448152274435739</v>
       </c>
       <c r="X29">
         <v>-0.0008782343627569134</v>
@@ -4504,7 +4504,7 @@
         <v>0.004371579665014336</v>
       </c>
       <c r="AB29">
-        <v>0.009527531083481477</v>
+        <v>0.009527531083481478</v>
       </c>
       <c r="AC29">
         <v>0.004225533836526463</v>
@@ -4519,16 +4519,16 @@
         <v>-0.003231763619575334</v>
       </c>
       <c r="AG29">
-        <v>0.004659026125931831</v>
+        <v>0.00987295071319072</v>
       </c>
       <c r="AH29">
         <v>0.008509481695206045</v>
       </c>
       <c r="AI29">
-        <v>0.0005202526941650021</v>
+        <v>0.0062100884644678</v>
       </c>
       <c r="AJ29">
-        <v>0.001870644904830243</v>
+        <v>0.009785435630689232</v>
       </c>
       <c r="AK29">
         <v>0.004659026125931165</v>
@@ -4592,31 +4592,31 @@
         <v>131.06</v>
       </c>
       <c r="H30">
-        <v>1.274206549158845</v>
+        <v>1.28305248311187</v>
       </c>
       <c r="I30">
-        <v>1.443068312403113</v>
+        <v>1.461420184512161</v>
       </c>
       <c r="J30">
-        <v>1.270663050804325</v>
+        <v>1.274181818181818</v>
       </c>
       <c r="K30">
         <v>0.005308051055473717</v>
       </c>
       <c r="L30">
-        <v>-1.554312234475219e-15</v>
+        <v>0.005674091857466923</v>
       </c>
       <c r="M30">
-        <v>2.664535259100376e-15</v>
+        <v>0.007952242774026175</v>
       </c>
       <c r="N30">
-        <v>-2.775557561562891e-15</v>
+        <v>0.005196984743626176</v>
       </c>
       <c r="O30">
         <v>127.417</v>
       </c>
       <c r="P30">
-        <v>19568.2109823866</v>
+        <v>19622.4</v>
       </c>
       <c r="Q30">
         <v>15400</v>
@@ -4667,16 +4667,16 @@
         <v>-0.00393700787401563</v>
       </c>
       <c r="AG30">
-        <v>0.004448270914045205</v>
+        <v>0.009668373253749918</v>
       </c>
       <c r="AH30">
         <v>0.008562069823368379</v>
       </c>
       <c r="AI30">
-        <v>0.0006685485069066743</v>
+        <v>0.006346433770014537</v>
       </c>
       <c r="AJ30">
-        <v>0.001820473323066452</v>
+        <v>0.009787192942918743</v>
       </c>
       <c r="AK30">
         <v>0.004448270914047869</v>
@@ -4685,7 +4685,7 @@
         <v>0.001431803212966321</v>
       </c>
       <c r="AM30">
-        <v>0.0006685485069082286</v>
+        <v>0.0006685485069082287</v>
       </c>
       <c r="AN30">
         <v>0.001820473323063787</v>
@@ -4740,31 +4740,31 @@
         <v>131.761</v>
       </c>
       <c r="H31">
-        <v>1.274206549158843</v>
+        <v>1.290356083086053</v>
       </c>
       <c r="I31">
-        <v>1.443068312403111</v>
+        <v>1.473001255755546</v>
       </c>
       <c r="J31">
-        <v>1.270663050804328</v>
+        <v>1.280826656837831</v>
       </c>
       <c r="K31">
         <v>0.005348695254081992</v>
       </c>
       <c r="L31">
-        <v>-1.887379141862766e-15</v>
+        <v>0.005692362604271084</v>
       </c>
       <c r="M31">
-        <v>-8.881784197001252e-16</v>
+        <v>0.007924532154488517</v>
       </c>
       <c r="N31">
-        <v>2.886579864025407e-15</v>
+        <v>0.00521498467580872</v>
       </c>
       <c r="O31">
         <v>128.082</v>
       </c>
       <c r="P31">
-        <v>19650.4228817737</v>
+        <v>19807.6</v>
       </c>
       <c r="Q31">
         <v>15464.7</v>
@@ -4779,7 +4779,7 @@
         <v>0.008532863053652529</v>
       </c>
       <c r="U31">
-        <v>0.01352916851720098</v>
+        <v>0.01352916851720099</v>
       </c>
       <c r="V31">
         <v>0.01996212938662145</v>
@@ -4815,16 +4815,16 @@
         <v>-0.0006975122064636352</v>
       </c>
       <c r="AG31">
-        <v>0.004201298701301592</v>
+        <v>0.009438193085453239</v>
       </c>
       <c r="AH31">
         <v>0.008551049353532569</v>
       </c>
       <c r="AI31">
-        <v>0.0006681018484133716</v>
+        <v>0.006364267530664103</v>
       </c>
       <c r="AJ31">
-        <v>0.001817165222252504</v>
+        <v>0.009756097560975618</v>
       </c>
       <c r="AK31">
         <v>0.004201298701298706</v>
@@ -4839,7 +4839,7 @@
         <v>0.001817165222253392</v>
       </c>
       <c r="AO31">
-        <v>-0.0006324903130576764</v>
+        <v>-0.0006324903130576765</v>
       </c>
       <c r="AP31">
         <v>0.01061034896500401</v>
@@ -4888,31 +4888,31 @@
         <v>132.462</v>
       </c>
       <c r="H32">
-        <v>1.274206549158848</v>
+        <v>1.297798205945585</v>
       </c>
       <c r="I32">
-        <v>1.443068312403111</v>
+        <v>1.484655740749338</v>
       </c>
       <c r="J32">
-        <v>1.270663050804325</v>
+        <v>1.287457365338825</v>
       </c>
       <c r="K32">
         <v>0.005320238917433828</v>
       </c>
       <c r="L32">
-        <v>4.218847493575595e-15</v>
+        <v>0.005767495466625583</v>
       </c>
       <c r="M32">
-        <v>-4.440892098500626e-16</v>
+        <v>0.007912067249266519</v>
       </c>
       <c r="N32">
-        <v>-2.997602166487923e-15</v>
+        <v>0.005176897643092815</v>
       </c>
       <c r="O32">
         <v>128.745</v>
       </c>
       <c r="P32">
-        <v>19744.8331464484</v>
+        <v>20005.8</v>
       </c>
       <c r="Q32">
         <v>15539</v>
@@ -4924,7 +4924,7 @@
         <v>0.01813669734257073</v>
       </c>
       <c r="T32">
-        <v>0.008460669320994318</v>
+        <v>0.008460669320994319</v>
       </c>
       <c r="U32">
         <v>0.01306313019248773</v>
@@ -4963,16 +4963,16 @@
         <v>-0.0006979990693346538</v>
       </c>
       <c r="AG32">
-        <v>0.004804490226124836</v>
+        <v>0.01000626022334861</v>
       </c>
       <c r="AH32">
         <v>0.008519311117904937</v>
       </c>
       <c r="AI32">
-        <v>0.0006676557863543042</v>
+        <v>0.006439001954696932</v>
       </c>
       <c r="AJ32">
-        <v>0.001767359657689926</v>
+        <v>0.009693410375422484</v>
       </c>
       <c r="AK32">
         <v>0.004804490226127944</v>
@@ -4987,7 +4987,7 @@
         <v>0.001767359657690371</v>
       </c>
       <c r="AO32">
-        <v>-0.0001146590102433231</v>
+        <v>-0.0001146590102433232</v>
       </c>
       <c r="AP32">
         <v>0</v>
@@ -5036,31 +5036,31 @@
         <v>133.169</v>
       </c>
       <c r="H33">
-        <v>1.274206549158843</v>
+        <v>1.30525301918945</v>
       </c>
       <c r="I33">
-        <v>1.44306831240311</v>
+        <v>1.496384872080089</v>
       </c>
       <c r="J33">
-        <v>1.27066305080433</v>
+        <v>1.294126313092493</v>
       </c>
       <c r="K33">
         <v>0.0053373797768419</v>
       </c>
       <c r="L33">
-        <v>-4.218847493575595e-15</v>
+        <v>0.005744200608162275</v>
       </c>
       <c r="M33">
-        <v>-6.661338147750939e-16</v>
+        <v>0.007900236404185357</v>
       </c>
       <c r="N33">
-        <v>4.440892098500626e-15</v>
+        <v>0.005179936775547622</v>
       </c>
       <c r="O33">
         <v>129.412</v>
       </c>
       <c r="P33">
-        <v>19837.5915491572</v>
+        <v>20203.9</v>
       </c>
       <c r="Q33">
         <v>15612</v>
@@ -5105,22 +5105,22 @@
         <v>0.005180783719756166</v>
       </c>
       <c r="AE33">
-        <v>0.006081292136293825</v>
+        <v>0.006081292136293826</v>
       </c>
       <c r="AF33">
         <v>0.0004656577415598218</v>
       </c>
       <c r="AG33">
-        <v>0.004697857004959616</v>
+        <v>0.00990212838276916</v>
       </c>
       <c r="AH33">
         <v>0.008487763474324561</v>
       </c>
       <c r="AI33">
-        <v>0.0005930758395689129</v>
+        <v>0.006340683194333341</v>
       </c>
       <c r="AJ33">
-        <v>0.00171781419750161</v>
+        <v>0.009631621739946139</v>
       </c>
       <c r="AK33">
         <v>0.004697857004955175</v>
@@ -5150,7 +5150,7 @@
         <v>0.007854246470898163</v>
       </c>
       <c r="AT33">
-        <v>0.01883421620432268</v>
+        <v>0.01883421620432269</v>
       </c>
       <c r="AU33">
         <v>309.205</v>
@@ -5184,31 +5184,31 @@
         <v>133.881</v>
       </c>
       <c r="H34">
-        <v>1.274206549158843</v>
+        <v>1.312800769971126</v>
       </c>
       <c r="I34">
-        <v>1.443068312403109</v>
+        <v>1.508166381344561</v>
       </c>
       <c r="J34">
-        <v>1.270663050804324</v>
+        <v>1.30084924065644</v>
       </c>
       <c r="K34">
         <v>0.005346589671770374</v>
       </c>
       <c r="L34">
-        <v>6.661338147750939e-16</v>
+        <v>0.005782595918731204</v>
       </c>
       <c r="M34">
-        <v>-6.661338147750939e-16</v>
+        <v>0.007873314869920378</v>
       </c>
       <c r="N34">
-        <v>-4.884981308350689e-15</v>
+        <v>0.005194954693318543</v>
       </c>
       <c r="O34">
         <v>130.084</v>
       </c>
       <c r="P34">
-        <v>19929.8416866455</v>
+        <v>20403.3</v>
       </c>
       <c r="Q34">
         <v>15684.6</v>
@@ -5217,7 +5217,7 @@
         <v>0.01399881380767742</v>
       </c>
       <c r="S34">
-        <v>0.01847694248759923</v>
+        <v>0.01847694248759924</v>
       </c>
       <c r="T34">
         <v>0.009662442792518711</v>
@@ -5226,7 +5226,7 @@
         <v>0.01532539945322786</v>
       </c>
       <c r="V34">
-        <v>0.01883421620432268</v>
+        <v>0.01883421620432269</v>
       </c>
       <c r="W34">
         <v>0.009517240447971087</v>
@@ -5259,16 +5259,16 @@
         <v>0.002792646032115487</v>
       </c>
       <c r="AG34">
-        <v>0.004650269023823039</v>
+        <v>0.009869381654036946</v>
       </c>
       <c r="AH34">
         <v>0.008536560928200654</v>
       </c>
       <c r="AI34">
-        <v>0.0007409053863829396</v>
+        <v>0.006527785661576857</v>
       </c>
       <c r="AJ34">
-        <v>0.001714868372264977</v>
+        <v>0.009601684940841126</v>
       </c>
       <c r="AK34">
         <v>0.004650269023827924</v>
@@ -5298,7 +5298,7 @@
         <v>0.01305112710759571</v>
       </c>
       <c r="AT34">
-        <v>0.007100643743468193</v>
+        <v>0.007100643743468194</v>
       </c>
       <c r="AU34">
         <v>311.088</v>
@@ -5332,31 +5332,31 @@
         <v>134.591</v>
       </c>
       <c r="H35">
-        <v>1.274206549158843</v>
+        <v>1.320363932243509</v>
       </c>
       <c r="I35">
-        <v>1.443068312403109</v>
+        <v>1.520070211095201</v>
       </c>
       <c r="J35">
-        <v>1.270663050804327</v>
+        <v>1.307566384315219</v>
       </c>
       <c r="K35">
         <v>0.005303217036024543</v>
       </c>
       <c r="L35">
-        <v>-3.33066907387547e-16</v>
+        <v>0.005761089150297494</v>
       </c>
       <c r="M35">
-        <v>-3.33066907387547e-16</v>
+        <v>0.00789291546203752</v>
       </c>
       <c r="N35">
-        <v>2.664535259100376e-15</v>
+        <v>0.005163660360357314</v>
       </c>
       <c r="O35">
         <v>130.756</v>
       </c>
       <c r="P35">
-        <v>20026.2850122016</v>
+        <v>20607.9</v>
       </c>
       <c r="Q35">
         <v>15760.5</v>
@@ -5374,7 +5374,7 @@
         <v>0.0149783389730509</v>
       </c>
       <c r="V35">
-        <v>0.007100643743468193</v>
+        <v>0.007100643743468194</v>
       </c>
       <c r="W35">
         <v>0.009427516506550937</v>
@@ -5407,16 +5407,16 @@
         <v>0.002552796472499397</v>
       </c>
       <c r="AG35">
-        <v>0.004839141578365957</v>
+        <v>0.01002778962226714</v>
       </c>
       <c r="AH35">
         <v>0.008523912654732069</v>
       </c>
       <c r="AI35">
-        <v>0.0008884282224028706</v>
+        <v>0.006654635686893728</v>
       </c>
       <c r="AJ35">
-        <v>0.001665664183592819</v>
+        <v>0.009571726592219942</v>
       </c>
       <c r="AK35">
         <v>0.004839141578363515</v>
@@ -5425,7 +5425,7 @@
         <v>0.001421949207974338</v>
       </c>
       <c r="AM35">
-        <v>0.0008884282224033146</v>
+        <v>0.0008884282224033147</v>
       </c>
       <c r="AN35">
         <v>0.001665664183593263</v>
@@ -5480,31 +5480,31 @@
         <v>135.301</v>
       </c>
       <c r="H36">
-        <v>1.274206549158846</v>
+        <v>1.327815548329885</v>
       </c>
       <c r="I36">
-        <v>1.443068312403113</v>
+        <v>1.531956100710136</v>
       </c>
       <c r="J36">
-        <v>1.270663050804326</v>
+        <v>1.314286616560349</v>
       </c>
       <c r="K36">
         <v>0.005275241286564425</v>
       </c>
       <c r="L36">
-        <v>1.998401444325282e-15</v>
+        <v>0.005643607723905486</v>
       </c>
       <c r="M36">
-        <v>2.886579864025407e-15</v>
+        <v>0.007819303034937608</v>
       </c>
       <c r="N36">
-        <v>-6.661338147750939e-16</v>
+        <v>0.0051394960330442</v>
       </c>
       <c r="O36">
         <v>131.429</v>
       </c>
       <c r="P36">
-        <v>20118.4080833849</v>
+        <v>20809.1</v>
       </c>
       <c r="Q36">
         <v>15833</v>
@@ -5516,7 +5516,7 @@
         <v>0.01781848041202072</v>
       </c>
       <c r="T36">
-        <v>0.009479257231096438</v>
+        <v>0.009479257231096439</v>
       </c>
       <c r="U36">
         <v>0.01462279385345244</v>
@@ -5528,7 +5528,7 @@
         <v>0.009339468512982396</v>
       </c>
       <c r="X36">
-        <v>0.001263840391369841</v>
+        <v>0.001263840391369842</v>
       </c>
       <c r="Y36">
         <v>-0.001744077801750121</v>
@@ -5543,7 +5543,7 @@
         <v>0.009528620759564399</v>
       </c>
       <c r="AC36">
-        <v>0.004245781062653275</v>
+        <v>0.004245781062653276</v>
       </c>
       <c r="AD36">
         <v>0.005146991342653395</v>
@@ -5555,16 +5555,16 @@
         <v>0.002314814814814659</v>
       </c>
       <c r="AG36">
-        <v>0.004600107864597636</v>
+        <v>0.009763246133764003</v>
       </c>
       <c r="AH36">
         <v>0.008491272311753617</v>
       </c>
       <c r="AI36">
-        <v>0.0009616095865099261</v>
+        <v>0.006610644257702969</v>
       </c>
       <c r="AJ36">
-        <v>0.001709085870019944</v>
+        <v>0.009541752765285017</v>
       </c>
       <c r="AK36">
         <v>0.004600107864598302</v>
@@ -5576,7 +5576,7 @@
         <v>0.0009616095865079277</v>
       </c>
       <c r="AN36">
-        <v>0.001709085870017057</v>
+        <v>0.001709085870017058</v>
       </c>
       <c r="AO36">
         <v>-0.004990364408904324</v>
@@ -5588,7 +5588,7 @@
         <v>0</v>
       </c>
       <c r="AR36">
-        <v>0.01640080485397521</v>
+        <v>0.01640080485397522</v>
       </c>
       <c r="AS36">
         <v>0.01212492312718294</v>
@@ -5628,31 +5628,31 @@
         <v>136.012</v>
       </c>
       <c r="H37">
-        <v>1.274206549158846</v>
+        <v>1.335400974745237</v>
       </c>
       <c r="I37">
-        <v>1.443068312403112</v>
+        <v>1.543918607862996</v>
       </c>
       <c r="J37">
-        <v>1.270663050804327</v>
+        <v>1.321034231243241</v>
       </c>
       <c r="K37">
         <v>0.005254950074278897</v>
       </c>
       <c r="L37">
-        <v>4.440892098500626e-16</v>
+        <v>0.005712710944598687</v>
       </c>
       <c r="M37">
-        <v>-4.440892098500626e-16</v>
+        <v>0.007808648790468054</v>
       </c>
       <c r="N37">
-        <v>6.661338147750939e-16</v>
+        <v>0.005134051125432082</v>
       </c>
       <c r="O37">
         <v>132.103</v>
       </c>
       <c r="P37">
-        <v>20208.1168947717</v>
+        <v>21009.2</v>
       </c>
       <c r="Q37">
         <v>15903.6</v>
@@ -5691,7 +5691,7 @@
         <v>0.009530864197530908</v>
       </c>
       <c r="AC37">
-        <v>0.004267925957276208</v>
+        <v>0.004267925957276209</v>
       </c>
       <c r="AD37">
         <v>0.005128244147029948</v>
@@ -5703,16 +5703,16 @@
         <v>0.005080831408776021</v>
       </c>
       <c r="AG37">
-        <v>0.00445904124297436</v>
+        <v>0.009615985314117559</v>
       </c>
       <c r="AH37">
         <v>0.008439313133681292</v>
       </c>
       <c r="AI37">
-        <v>0.0007389890629625473</v>
+        <v>0.006455921638468531</v>
       </c>
       <c r="AJ37">
-        <v>0.001660057179746932</v>
+        <v>0.009481668773704266</v>
       </c>
       <c r="AK37">
         <v>0.004459041242973472</v>
@@ -5776,37 +5776,37 @@
         <v>136.723</v>
       </c>
       <c r="H38">
-        <v>1.274206549158847</v>
+        <v>1.342901416765053</v>
       </c>
       <c r="I38">
-        <v>1.443068312403111</v>
+        <v>1.55581598419045</v>
       </c>
       <c r="J38">
-        <v>1.27066305080433</v>
+        <v>1.32777374455515</v>
       </c>
       <c r="K38">
         <v>0.005227479928241685</v>
       </c>
       <c r="L38">
-        <v>6.661338147750939e-16</v>
+        <v>0.005616621645230691</v>
       </c>
       <c r="M38">
-        <v>-4.440892098500626e-16</v>
+        <v>0.007705960836835502</v>
       </c>
       <c r="N38">
-        <v>1.77635683940025e-15</v>
+        <v>0.005101694681723945</v>
       </c>
       <c r="O38">
         <v>132.778</v>
       </c>
       <c r="P38">
-        <v>20303.1624909719</v>
+        <v>21215.7</v>
       </c>
       <c r="Q38">
         <v>15978.4</v>
       </c>
       <c r="R38">
-        <v>0.0139986879179903</v>
+        <v>0.01399868791799031</v>
       </c>
       <c r="S38">
         <v>0.01793351530969023</v>
@@ -5824,7 +5824,7 @@
         <v>0.009337335257183055</v>
       </c>
       <c r="X38">
-        <v>1.399313064487373e-05</v>
+        <v>1.399313064487373e-005</v>
       </c>
       <c r="Y38">
         <v>0.001360032091262342</v>
@@ -5851,22 +5851,22 @@
         <v>0.005974264705882248</v>
       </c>
       <c r="AG38">
-        <v>0.004703337609096581</v>
+        <v>0.009829027283285496</v>
       </c>
       <c r="AH38">
         <v>0.008349315201177765</v>
       </c>
       <c r="AI38">
-        <v>0.000738443361394836</v>
+        <v>0.006359212563592065</v>
       </c>
       <c r="AJ38">
-        <v>0.001703342233679628</v>
+        <v>0.009422428959060314</v>
       </c>
       <c r="AK38">
         <v>0.004703337609094804</v>
       </c>
       <c r="AL38">
-        <v>0.001331029990654597</v>
+        <v>0.001331029990654598</v>
       </c>
       <c r="AM38">
         <v>0.0007384433613941699</v>
@@ -5924,31 +5924,31 @@
         <v>137.433</v>
       </c>
       <c r="H39">
-        <v>1.274206549158849</v>
+        <v>1.350442477876106</v>
       </c>
       <c r="I39">
-        <v>1.443068312403111</v>
+        <v>1.567836659784354</v>
       </c>
       <c r="J39">
-        <v>1.270663050804329</v>
+        <v>1.334539949160146</v>
       </c>
       <c r="K39">
         <v>0.00519298142960567</v>
       </c>
       <c r="L39">
-        <v>1.77635683940025e-15</v>
+        <v>0.005615498663497309</v>
       </c>
       <c r="M39">
-        <v>-3.33066907387547e-16</v>
+        <v>0.007726283645401066</v>
       </c>
       <c r="N39">
-        <v>-5.551115123125783e-16</v>
+        <v>0.005095901792562474</v>
       </c>
       <c r="O39">
         <v>133.454</v>
       </c>
       <c r="P39">
-        <v>20394.6502306298</v>
+        <v>21419.9</v>
       </c>
       <c r="Q39">
         <v>16050.4</v>
@@ -5972,7 +5972,7 @@
         <v>0.009250955979750453</v>
       </c>
       <c r="X39">
-        <v>1.399293484016795e-05</v>
+        <v>1.399293484016795e-005</v>
       </c>
       <c r="Y39">
         <v>0.00135818491619033</v>
@@ -5999,16 +5999,16 @@
         <v>0.006167199634536269</v>
       </c>
       <c r="AG39">
-        <v>0.004506083212336032</v>
+        <v>0.009624947562418385</v>
       </c>
       <c r="AH39">
         <v>0.00828018135710451</v>
       </c>
       <c r="AI39">
-        <v>0.0005903187721385539</v>
+        <v>0.006209132369910497</v>
       </c>
       <c r="AJ39">
-        <v>0.001654487798152138</v>
+        <v>0.009393554485569888</v>
       </c>
       <c r="AK39">
         <v>0.004506083212336698</v>
@@ -6026,7 +6026,7 @@
         <v>-0.004912063372836228</v>
       </c>
       <c r="AP39">
-        <v>-0.01564172677114894</v>
+        <v>-0.01564172677114895</v>
       </c>
       <c r="AQ39">
         <v>0</v>
@@ -6072,31 +6072,31 @@
         <v>138.145</v>
       </c>
       <c r="H40">
-        <v>1.274206549158847</v>
+        <v>1.357948264426266</v>
       </c>
       <c r="I40">
-        <v>1.44306831240311</v>
+        <v>1.5798176904402</v>
       </c>
       <c r="J40">
-        <v>1.270663050804325</v>
+        <v>1.341306855533918</v>
       </c>
       <c r="K40">
-        <v>0.00518070623503819</v>
+        <v>0.005180706235038191</v>
       </c>
       <c r="L40">
-        <v>-1.77635683940025e-15</v>
+        <v>0.005558020184587287</v>
       </c>
       <c r="M40">
-        <v>-4.440892098500626e-16</v>
+        <v>0.007641759478626886</v>
       </c>
       <c r="N40">
-        <v>-2.997602166487923e-15</v>
+        <v>0.005070591088734755</v>
       </c>
       <c r="O40">
         <v>134.131</v>
       </c>
       <c r="P40">
-        <v>20488.4251637791</v>
+        <v>21627.5</v>
       </c>
       <c r="Q40">
         <v>16124.2</v>
@@ -6120,7 +6120,7 @@
         <v>0.009166160234914011</v>
       </c>
       <c r="X40">
-        <v>1.399273904056919e-05</v>
+        <v>1.399273904056919e-005</v>
       </c>
       <c r="Y40">
         <v>0.001356342751923645</v>
@@ -6138,34 +6138,34 @@
         <v>0.004305889700610965</v>
       </c>
       <c r="AD40">
-        <v>0.005072909017339144</v>
+        <v>0.005072909017339145</v>
       </c>
       <c r="AE40">
-        <v>0.005899990327884685</v>
+        <v>0.005899990327884686</v>
       </c>
       <c r="AF40">
         <v>0.006129398410896769</v>
       </c>
       <c r="AG40">
-        <v>0.004598016248813286</v>
+        <v>0.009691921997768471</v>
       </c>
       <c r="AH40">
         <v>0.008250290570279928</v>
       </c>
       <c r="AI40">
-        <v>0.0006637168141576666</v>
+        <v>0.006225425950196595</v>
       </c>
       <c r="AJ40">
-        <v>0.00165175498967618</v>
+        <v>0.009306136782651908</v>
       </c>
       <c r="AK40">
-        <v>0.004598016248816394</v>
+        <v>0.004598016248816395</v>
       </c>
       <c r="AL40">
         <v>0.001299288216020766</v>
       </c>
       <c r="AM40">
-        <v>0.0006637168141594429</v>
+        <v>0.000663716814159443</v>
       </c>
       <c r="AN40">
         <v>0.001651754989676402</v>
@@ -6220,31 +6220,31 @@
         <v>138.86</v>
       </c>
       <c r="H41">
-        <v>1.274206549158847</v>
+        <v>1.365571596935769</v>
       </c>
       <c r="I41">
-        <v>1.44306831240311</v>
+        <v>1.59194219600311</v>
       </c>
       <c r="J41">
-        <v>1.270663050804327</v>
+        <v>1.348092668288527</v>
       </c>
       <c r="K41">
         <v>0.00517572116254672</v>
       </c>
       <c r="L41">
-        <v>-5.551115123125783e-16</v>
+        <v>0.005613860784839497</v>
       </c>
       <c r="M41">
-        <v>-3.33066907387547e-16</v>
+        <v>0.007674623240566003</v>
       </c>
       <c r="N41">
-        <v>1.77635683940025e-15</v>
+        <v>0.00505910539904586</v>
       </c>
       <c r="O41">
         <v>134.809</v>
       </c>
       <c r="P41">
-        <v>20578.8963729964</v>
+        <v>21832.9</v>
       </c>
       <c r="Q41">
         <v>16195.4</v>
@@ -6253,7 +6253,7 @@
         <v>0.0134344921299967</v>
       </c>
       <c r="S41">
-        <v>0.01701794080385421</v>
+        <v>0.01701794080385422</v>
       </c>
       <c r="T41">
         <v>0.01332616084309368</v>
@@ -6268,7 +6268,7 @@
         <v>0.009082904873445541</v>
       </c>
       <c r="X41">
-        <v>1.399254324652155e-05</v>
+        <v>1.399254324652155e-005</v>
       </c>
       <c r="Y41">
         <v>0.001354505578100351</v>
@@ -6295,16 +6295,16 @@
         <v>0.005866425992779645</v>
       </c>
       <c r="AG41">
-        <v>0.004415722950597667</v>
+        <v>0.009497167957461583</v>
       </c>
       <c r="AH41">
         <v>0.008201678131378065</v>
       </c>
       <c r="AI41">
-        <v>0.000515881789372008</v>
+        <v>0.006132638662759149</v>
       </c>
       <c r="AJ41">
-        <v>0.001649031194173034</v>
+        <v>0.009336310127866732</v>
       </c>
       <c r="AK41">
         <v>0.004415722950595891</v>
@@ -6313,7 +6313,7 @@
         <v>0.00124118476727797</v>
       </c>
       <c r="AM41">
-        <v>0.0005158817893726741</v>
+        <v>0.0005158817893726742</v>
       </c>
       <c r="AN41">
         <v>0.001649031194173478</v>
@@ -6368,31 +6368,31 @@
         <v>139.577</v>
       </c>
       <c r="H42">
-        <v>1.274206549158846</v>
+        <v>1.373260693513951</v>
       </c>
       <c r="I42">
-        <v>1.443068312403109</v>
+        <v>1.604072501483815</v>
       </c>
       <c r="J42">
-        <v>1.270663050804328</v>
+        <v>1.354895029662189</v>
       </c>
       <c r="K42">
-        <v>0.005163474002592316</v>
+        <v>0.005163474002592317</v>
       </c>
       <c r="L42">
-        <v>-6.661338147750939e-16</v>
+        <v>0.005630679925853643</v>
       </c>
       <c r="M42">
-        <v>-4.440892098500626e-16</v>
+        <v>0.007619815286736387</v>
       </c>
       <c r="N42">
-        <v>4.440892098500626e-16</v>
+        <v>0.005045915265082357</v>
       </c>
       <c r="O42">
         <v>135.489</v>
       </c>
       <c r="P42">
-        <v>20669.2405159086</v>
+        <v>22039.4</v>
       </c>
       <c r="Q42">
         <v>16266.5</v>
@@ -6416,7 +6416,7 @@
         <v>0.008972931533858031</v>
       </c>
       <c r="X42">
-        <v>-8.141002157358024e-05</v>
+        <v>-8.141002157358024e-005</v>
       </c>
       <c r="Y42">
         <v>0.003123445791956225</v>
@@ -6443,16 +6443,16 @@
         <v>0.00605652759084796</v>
       </c>
       <c r="AG42">
-        <v>0.004390135470566214</v>
+        <v>0.009458202987234765</v>
       </c>
       <c r="AH42">
         <v>0.008191190253045821</v>
       </c>
       <c r="AI42">
-        <v>0.0005156157925745308</v>
+        <v>0.006149198985921478</v>
       </c>
       <c r="AJ42">
-        <v>0.001646316367128087</v>
+        <v>0.009278676280486176</v>
       </c>
       <c r="AK42">
         <v>0.00439013547056577</v>
@@ -6516,31 +6516,31 @@
         <v>140.297</v>
       </c>
       <c r="H43">
-        <v>1.274206549158845</v>
+        <v>1.380941869021339</v>
       </c>
       <c r="I43">
-        <v>1.443068312403109</v>
+        <v>1.616299740188705</v>
       </c>
       <c r="J43">
-        <v>1.27066305080433</v>
+        <v>1.36171554135527</v>
       </c>
       <c r="K43">
         <v>0.005158443009951386</v>
       </c>
       <c r="L43">
-        <v>-8.881784197001252e-16</v>
+        <v>0.00559338481299787</v>
       </c>
       <c r="M43">
-        <v>-4.440892098500626e-16</v>
+        <v>0.007622622227847931</v>
       </c>
       <c r="N43">
-        <v>1.332267629550188e-15</v>
+        <v>0.005033977942026535</v>
       </c>
       <c r="O43">
         <v>136.171</v>
       </c>
       <c r="P43">
-        <v>20759.7117251259</v>
+        <v>22247.3</v>
       </c>
       <c r="Q43">
         <v>16337.7</v>
@@ -6564,7 +6564,7 @@
         <v>0.008893134050897755</v>
       </c>
       <c r="X43">
-        <v>-8.14166497048463e-05</v>
+        <v>-8.14166497048463e-005</v>
       </c>
       <c r="Y43">
         <v>0.003113720255526475</v>
@@ -6591,16 +6591,16 @@
         <v>0.005797101449275255</v>
       </c>
       <c r="AG43">
-        <v>0.004377094027604223</v>
+        <v>0.009433106164414618</v>
       </c>
       <c r="AH43">
         <v>0.008180415341997094</v>
       </c>
       <c r="AI43">
-        <v>0.0005153500699395241</v>
+        <v>0.006111617434192862</v>
       </c>
       <c r="AJ43">
-        <v>0.0016436104643196</v>
+        <v>0.009278761313826989</v>
       </c>
       <c r="AK43">
         <v>0.00437709402760289</v>
@@ -6664,31 +6664,31 @@
         <v>141.018</v>
       </c>
       <c r="H44">
-        <v>1.274206549158847</v>
+        <v>1.388586556846595</v>
       </c>
       <c r="I44">
-        <v>1.443068312403113</v>
+        <v>1.628577929465302</v>
       </c>
       <c r="J44">
-        <v>1.270663050804329</v>
+        <v>1.368543256222119</v>
       </c>
       <c r="K44">
         <v>0.005139097771156953</v>
       </c>
       <c r="L44">
-        <v>1.77635683940025e-15</v>
+        <v>0.005535850564566847</v>
       </c>
       <c r="M44">
-        <v>2.886579864025407e-15</v>
+        <v>0.007596480387457749</v>
       </c>
       <c r="N44">
-        <v>-5.551115123125783e-16</v>
+        <v>0.00501405371348973</v>
       </c>
       <c r="O44">
         <v>136.854</v>
       </c>
       <c r="P44">
-        <v>20850.5641332584</v>
+        <v>22456.7</v>
       </c>
       <c r="Q44">
         <v>16409.2</v>
@@ -6712,7 +6712,7 @@
         <v>0.008814743356603261</v>
       </c>
       <c r="X44">
-        <v>-8.142327891558221e-05</v>
+        <v>-8.142327891558221e-005</v>
       </c>
       <c r="Y44">
         <v>0.003104055096298852</v>
@@ -6730,7 +6730,7 @@
         <v>0.004245954020900999</v>
       </c>
       <c r="AD44">
-        <v>0.005015752252682359</v>
+        <v>0.00501575225268236</v>
       </c>
       <c r="AE44">
         <v>0.005794230153771229</v>
@@ -6739,16 +6739,16 @@
         <v>0.005098647749944618</v>
       </c>
       <c r="AG44">
-        <v>0.004376381008342145</v>
+        <v>0.009412378131278931</v>
       </c>
       <c r="AH44">
         <v>0.008187803123905102</v>
       </c>
       <c r="AI44">
-        <v>0.0005886681383386883</v>
+        <v>0.006127777481749863</v>
       </c>
       <c r="AJ44">
-        <v>0.001640913441818714</v>
+        <v>0.009249858996051907</v>
       </c>
       <c r="AK44">
         <v>0.004376381008342589</v>
@@ -6812,31 +6812,31 @@
         <v>141.741</v>
       </c>
       <c r="H45">
-        <v>1.274206549158849</v>
+        <v>1.396295751874173</v>
       </c>
       <c r="I45">
-        <v>1.443068312403112</v>
+        <v>1.640952251147154</v>
       </c>
       <c r="J45">
-        <v>1.270663050804328</v>
+        <v>1.375384279555418</v>
       </c>
       <c r="K45">
         <v>0.005127005063183532</v>
       </c>
       <c r="L45">
-        <v>1.77635683940025e-15</v>
+        <v>0.005551828936818382</v>
       </c>
       <c r="M45">
-        <v>-3.33066907387547e-16</v>
+        <v>0.007598237368914296</v>
       </c>
       <c r="N45">
-        <v>-6.661338147750939e-16</v>
+        <v>0.004998762956301084</v>
       </c>
       <c r="O45">
         <v>137.538</v>
       </c>
       <c r="P45">
-        <v>20955.6479675599</v>
+        <v>22682.7</v>
       </c>
       <c r="Q45">
         <v>16491.9</v>
@@ -6860,7 +6860,7 @@
         <v>0.008737722574587048</v>
       </c>
       <c r="X45">
-        <v>-8.142990920556592e-05</v>
+        <v>-8.142990920556592e-005</v>
       </c>
       <c r="Y45">
         <v>0.003094449753770601</v>
@@ -6887,16 +6887,16 @@
         <v>0.002646669607410779</v>
       </c>
       <c r="AG45">
-        <v>0.005039855690709416</v>
+        <v>0.01006381169094306</v>
       </c>
       <c r="AH45">
         <v>0.00815788992335964</v>
       </c>
       <c r="AI45">
-        <v>0.0005883218120328326</v>
+        <v>0.006143417010909813</v>
       </c>
       <c r="AJ45">
-        <v>0.001638225255972348</v>
+        <v>0.009248910249245457</v>
       </c>
       <c r="AK45">
         <v>0.005039855690710082</v>
@@ -6923,7 +6923,7 @@
         <v>0.01542535619014784</v>
       </c>
       <c r="AS45">
-        <v>0.01079838302637492</v>
+        <v>0.01079838302637493</v>
       </c>
       <c r="AT45">
         <v>0.009093902522441688</v>
@@ -6960,31 +6960,31 @@
         <v>142.466</v>
       </c>
       <c r="H46">
-        <v>1.274206549158848</v>
+        <v>1.404172482186146</v>
       </c>
       <c r="I46">
-        <v>1.443068312403112</v>
+        <v>1.653467591962625</v>
       </c>
       <c r="J46">
-        <v>1.270663050804328</v>
+        <v>1.382244157912838</v>
       </c>
       <c r="K46">
         <v>0.005114963207540457</v>
       </c>
       <c r="L46">
-        <v>-6.661338147750939e-16</v>
+        <v>0.00564116183938812</v>
       </c>
       <c r="M46">
-        <v>-4.440892098500626e-16</v>
+        <v>0.007626876898290336</v>
       </c>
       <c r="N46">
-        <v>2.220446049250313e-16</v>
+        <v>0.004987608524678722</v>
       </c>
       <c r="O46">
         <v>138.224</v>
       </c>
       <c r="P46">
-        <v>21059.5882051157</v>
+        <v>22908.9</v>
       </c>
       <c r="Q46">
         <v>16573.7</v>
@@ -7035,16 +7035,16 @@
         <v>-0.0002199736031677224</v>
       </c>
       <c r="AG46">
-        <v>0.004960010671905879</v>
+        <v>0.009972357788094133</v>
       </c>
       <c r="AH46">
         <v>0.008200736614837556</v>
       </c>
       <c r="AI46">
-        <v>0.0005144789063642463</v>
+        <v>0.006158543004526784</v>
       </c>
       <c r="AJ46">
-        <v>0.00163554586343162</v>
+        <v>0.009274896868683991</v>
       </c>
       <c r="AK46">
         <v>0.004960010671905657</v>
@@ -7053,7 +7053,7 @@
         <v>0.001261458245731983</v>
       </c>
       <c r="AM46">
-        <v>0.0005144789063649124</v>
+        <v>0.0005144789063649125</v>
       </c>
       <c r="AN46">
         <v>0.001635545863431842</v>
@@ -7108,31 +7108,31 @@
         <v>143.193</v>
       </c>
       <c r="H47">
-        <v>1.274206549158847</v>
+        <v>1.412114537444934</v>
       </c>
       <c r="I47">
-        <v>1.443068312403111</v>
+        <v>1.666077978535525</v>
       </c>
       <c r="J47">
-        <v>1.270663050804329</v>
+        <v>1.389120710876287</v>
       </c>
       <c r="K47">
         <v>0.005102971937164025</v>
       </c>
       <c r="L47">
-        <v>-5.551115123125783e-16</v>
+        <v>0.005656039667166324</v>
       </c>
       <c r="M47">
-        <v>-4.440892098500626e-16</v>
+        <v>0.007626630624148589</v>
       </c>
       <c r="N47">
-        <v>4.440892098500626e-16</v>
+        <v>0.004974919173348136</v>
       </c>
       <c r="O47">
         <v>138.911</v>
       </c>
       <c r="P47">
-        <v>21163.5284426715</v>
+        <v>23136.5</v>
       </c>
       <c r="Q47">
         <v>16655.5</v>
@@ -7183,16 +7183,16 @@
         <v>-0.0008800880088007945</v>
       </c>
       <c r="AG47">
-        <v>0.00493553038850747</v>
+        <v>0.009935003426615685</v>
       </c>
       <c r="AH47">
         <v>0.008188018499523109</v>
       </c>
       <c r="AI47">
-        <v>0.0005142143539258459</v>
+        <v>0.006173162437876023</v>
       </c>
       <c r="AJ47">
-        <v>0.001632875221118102</v>
+        <v>0.009271959181434086</v>
       </c>
       <c r="AK47">
         <v>0.004935530388507026</v>
@@ -7201,7 +7201,7 @@
         <v>0.001259868973626732</v>
       </c>
       <c r="AM47">
-        <v>0.000514214353926512</v>
+        <v>0.0005142143539265121</v>
       </c>
       <c r="AN47">
         <v>0.001632875221118768</v>
@@ -7219,7 +7219,7 @@
         <v>0.01478551665123629</v>
       </c>
       <c r="AS47">
-        <v>0.01045203715713749</v>
+        <v>0.0104520371571375</v>
       </c>
       <c r="AT47">
         <v>0.009503338170518516</v>
@@ -7256,31 +7256,31 @@
         <v>143.922</v>
       </c>
       <c r="H48">
-        <v>1.274206549158846</v>
+        <v>1.420048433257503</v>
       </c>
       <c r="I48">
-        <v>1.443068312403111</v>
+        <v>1.678737736787377</v>
       </c>
       <c r="J48">
-        <v>1.270663050804328</v>
+        <v>1.395998733549586</v>
       </c>
       <c r="K48">
         <v>0.005091030986151379</v>
       </c>
       <c r="L48">
-        <v>-8.881784197001252e-16</v>
+        <v>0.005618450630020977</v>
       </c>
       <c r="M48">
-        <v>-3.33066907387547e-16</v>
+        <v>0.007598538852893411</v>
       </c>
       <c r="N48">
-        <v>-9.992007221626409e-16</v>
+        <v>0.004951349885899958</v>
       </c>
       <c r="O48">
         <v>139.6</v>
       </c>
       <c r="P48">
-        <v>21270.5182715492</v>
+        <v>23368.6</v>
       </c>
       <c r="Q48">
         <v>16739.7</v>
@@ -7331,16 +7331,16 @@
         <v>-0.0008808632459811339</v>
       </c>
       <c r="AG48">
-        <v>0.005055387109362153</v>
+        <v>0.01003176798565031</v>
       </c>
       <c r="AH48">
         <v>0.00819291732114813</v>
       </c>
       <c r="AI48">
-        <v>0.0005139500734205882</v>
+        <v>0.006135288306556408</v>
       </c>
       <c r="AJ48">
-        <v>0.001630213286237803</v>
+        <v>0.009241139378125762</v>
       </c>
       <c r="AK48">
         <v>0.005055387109363263</v>
@@ -7404,31 +7404,31 @@
         <v>144.654</v>
       </c>
       <c r="H49">
-        <v>1.274206549158845</v>
+        <v>1.428120874284876</v>
       </c>
       <c r="I49">
-        <v>1.44306831240311</v>
+        <v>1.69149176258181</v>
       </c>
       <c r="J49">
-        <v>1.270663050804329</v>
+        <v>1.402904339866018</v>
       </c>
       <c r="K49">
         <v>0.005086088297828084</v>
       </c>
       <c r="L49">
-        <v>-6.661338147750939e-16</v>
+        <v>0.00568462373417411</v>
       </c>
       <c r="M49">
-        <v>-3.33066907387547e-16</v>
+        <v>0.007597390298046403</v>
       </c>
       <c r="N49">
-        <v>1.110223024625157e-15</v>
+        <v>0.004946713883380971</v>
       </c>
       <c r="O49">
         <v>140.29</v>
       </c>
       <c r="P49">
-        <v>21376.4915699863</v>
+        <v>23601.2</v>
       </c>
       <c r="Q49">
         <v>16823.1</v>
@@ -7476,19 +7476,19 @@
         <v>0.005686850047834646</v>
       </c>
       <c r="AF49">
-        <v>-0.001102049812651495</v>
+        <v>-0.001102049812651496</v>
       </c>
       <c r="AG49">
-        <v>0.004982168139214815</v>
+        <v>0.009953527382898564</v>
       </c>
       <c r="AH49">
         <v>0.008197156666607697</v>
       </c>
       <c r="AI49">
-        <v>0.0005136860644303631</v>
+        <v>0.006201229910598904</v>
       </c>
       <c r="AJ49">
-        <v>0.001627560016275176</v>
+        <v>0.009237315522999001</v>
       </c>
       <c r="AK49">
         <v>0.004982168139213927</v>

</xml_diff>